<commit_message>
updating league skins page
</commit_message>
<xml_diff>
--- a/LeagueSkins.xlsx
+++ b/LeagueSkins.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Blaze5545" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="389">
   <si>
     <t>Champion</t>
   </si>
@@ -40,9 +40,6 @@
     <t>Crimson Akali</t>
   </si>
   <si>
-    <t>All-Star Akali</t>
-  </si>
-  <si>
     <t>Blood Moon Akali</t>
   </si>
   <si>
@@ -58,9 +55,6 @@
     <t>Amumu</t>
   </si>
   <si>
-    <t>Pharoh Amumu</t>
-  </si>
-  <si>
     <t>Sad Robot Amumu</t>
   </si>
   <si>
@@ -571,9 +565,6 @@
     <t>Nasus</t>
   </si>
   <si>
-    <t>Galatic Nasus</t>
-  </si>
-  <si>
     <t>Infernal Nasus</t>
   </si>
   <si>
@@ -1078,9 +1069,6 @@
     <t>AstroNautilus</t>
   </si>
   <si>
-    <t>Lolipoppy</t>
-  </si>
-  <si>
     <t>Riot Girl Tristana</t>
   </si>
   <si>
@@ -1145,6 +1133,54 @@
   </si>
   <si>
     <t>Urf the Nami-tee</t>
+  </si>
+  <si>
+    <t>Xayah</t>
+  </si>
+  <si>
+    <t>Rakan</t>
+  </si>
+  <si>
+    <t>Ashen Lord Aurelion Sol</t>
+  </si>
+  <si>
+    <t>Lucian Prime</t>
+  </si>
+  <si>
+    <t>Astronaut Teemo</t>
+  </si>
+  <si>
+    <t>Star Guardian Jinx</t>
+  </si>
+  <si>
+    <t>All-star Akali</t>
+  </si>
+  <si>
+    <t>Pharaoh Amumu</t>
+  </si>
+  <si>
+    <t>Conqueror Karma</t>
+  </si>
+  <si>
+    <t>Galactic Nasus</t>
+  </si>
+  <si>
+    <t>Lollipoppy</t>
+  </si>
+  <si>
+    <t>Master Chef Tahm Kench</t>
+  </si>
+  <si>
+    <t>Nurse Akali</t>
+  </si>
+  <si>
+    <t>Worldbreaker Trundle</t>
+  </si>
+  <si>
+    <t>Boneclaw Shyvana</t>
+  </si>
+  <si>
+    <t>Super Galaxy Shyvana</t>
   </si>
 </sst>
 </file>
@@ -1484,24 +1520,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J135"/>
+  <dimension ref="A1:J137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -1536,1373 +1572,1413 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
+        <v>379</v>
+      </c>
+      <c r="D4" t="s">
+        <v>385</v>
+      </c>
+      <c r="E4" t="s">
         <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>380</v>
+      </c>
+      <c r="C6" t="s">
         <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
         <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8" t="s">
+        <v>343</v>
+      </c>
+      <c r="E8" t="s">
         <v>20</v>
       </c>
-      <c r="C8" t="s">
+      <c r="F8" t="s">
         <v>21</v>
       </c>
-      <c r="D8" t="s">
-        <v>346</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>22</v>
       </c>
-      <c r="F8" t="s">
+      <c r="H8" t="s">
+        <v>344</v>
+      </c>
+      <c r="I8" t="s">
         <v>23</v>
       </c>
-      <c r="G8" t="s">
+      <c r="J8" t="s">
         <v>24</v>
-      </c>
-      <c r="H8" t="s">
-        <v>347</v>
-      </c>
-      <c r="I8" t="s">
-        <v>25</v>
-      </c>
-      <c r="J8" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
         <v>27</v>
-      </c>
-      <c r="B9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
         <v>32</v>
-      </c>
-      <c r="B12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
         <v>35</v>
       </c>
-      <c r="B13" t="s">
+      <c r="D13" t="s">
         <v>36</v>
       </c>
-      <c r="C13" t="s">
+      <c r="E13" t="s">
         <v>37</v>
-      </c>
-      <c r="D13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
         <v>44</v>
-      </c>
-      <c r="B16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" t="s">
         <v>51</v>
       </c>
-      <c r="B20" t="s">
+      <c r="D20" t="s">
         <v>52</v>
       </c>
-      <c r="C20" t="s">
+      <c r="E20" t="s">
         <v>53</v>
-      </c>
-      <c r="D20" t="s">
-        <v>54</v>
-      </c>
-      <c r="E20" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B23" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C23" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D23" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="E23" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" t="s">
         <v>62</v>
       </c>
-      <c r="B24" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" t="s">
-        <v>64</v>
-      </c>
       <c r="D24" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="B27" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="C27" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" t="s">
         <v>68</v>
       </c>
-      <c r="B28" t="s">
+      <c r="D28" t="s">
         <v>69</v>
       </c>
-      <c r="C28" t="s">
+      <c r="E28" t="s">
         <v>70</v>
       </c>
-      <c r="D28" t="s">
+      <c r="F28" t="s">
         <v>71</v>
       </c>
-      <c r="E28" t="s">
+      <c r="G28" t="s">
         <v>72</v>
-      </c>
-      <c r="F28" t="s">
-        <v>73</v>
-      </c>
-      <c r="G28" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" t="s">
         <v>75</v>
       </c>
-      <c r="B29" t="s">
+      <c r="D29" t="s">
         <v>76</v>
-      </c>
-      <c r="C29" t="s">
-        <v>77</v>
-      </c>
-      <c r="D29" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B31" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" t="s">
+        <v>82</v>
+      </c>
+      <c r="C32" t="s">
         <v>83</v>
-      </c>
-      <c r="B32" t="s">
-        <v>84</v>
-      </c>
-      <c r="C32" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" t="s">
         <v>86</v>
       </c>
-      <c r="B33" t="s">
+      <c r="D33" t="s">
         <v>87</v>
-      </c>
-      <c r="C33" t="s">
-        <v>88</v>
-      </c>
-      <c r="D33" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" t="s">
         <v>90</v>
-      </c>
-      <c r="B34" t="s">
-        <v>91</v>
-      </c>
-      <c r="C34" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B35" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
+        <v>92</v>
+      </c>
+      <c r="B36" t="s">
+        <v>93</v>
+      </c>
+      <c r="C36" t="s">
         <v>94</v>
       </c>
-      <c r="B36" t="s">
-        <v>95</v>
-      </c>
-      <c r="C36" t="s">
-        <v>96</v>
-      </c>
       <c r="D36" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B37" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
+        <v>97</v>
+      </c>
+      <c r="B38" t="s">
+        <v>98</v>
+      </c>
+      <c r="C38" t="s">
         <v>99</v>
-      </c>
-      <c r="B38" t="s">
-        <v>100</v>
-      </c>
-      <c r="C38" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B39" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C39" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B40" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B41" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="B42" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B43" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B44" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
+        <v>109</v>
+      </c>
+      <c r="B45" t="s">
+        <v>110</v>
+      </c>
+      <c r="C45" t="s">
         <v>111</v>
-      </c>
-      <c r="B45" t="s">
-        <v>112</v>
-      </c>
-      <c r="C45" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B46" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B47" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B48" t="s">
-        <v>119</v>
+        <v>117</v>
+      </c>
+      <c r="C48" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B49" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B50" t="s">
-        <v>123</v>
+        <v>121</v>
+      </c>
+      <c r="C50" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B51" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" t="s">
+        <v>124</v>
+      </c>
+      <c r="B52" t="s">
+        <v>125</v>
+      </c>
+      <c r="C52" t="s">
         <v>126</v>
-      </c>
-      <c r="B52" t="s">
-        <v>127</v>
-      </c>
-      <c r="C52" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" t="s">
+        <v>127</v>
+      </c>
+      <c r="B53" t="s">
+        <v>128</v>
+      </c>
+      <c r="C53" t="s">
         <v>129</v>
-      </c>
-      <c r="B53" t="s">
-        <v>130</v>
-      </c>
-      <c r="C53" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" t="s">
+        <v>130</v>
+      </c>
+      <c r="B54" t="s">
+        <v>131</v>
+      </c>
+      <c r="C54" t="s">
         <v>132</v>
       </c>
-      <c r="B54" t="s">
+      <c r="D54" t="s">
         <v>133</v>
       </c>
-      <c r="C54" t="s">
+      <c r="E54" t="s">
         <v>134</v>
-      </c>
-      <c r="D54" t="s">
-        <v>135</v>
-      </c>
-      <c r="E54" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B55" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B56" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" t="s">
+        <v>140</v>
+      </c>
+      <c r="B59" t="s">
+        <v>141</v>
+      </c>
+      <c r="C59" t="s">
         <v>142</v>
       </c>
-      <c r="B59" t="s">
+      <c r="D59" t="s">
         <v>143</v>
-      </c>
-      <c r="C59" t="s">
-        <v>144</v>
-      </c>
-      <c r="D59" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B60" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B61" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B62" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B63" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" t="s">
-        <v>154</v>
+        <v>152</v>
+      </c>
+      <c r="B64" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" t="s">
+        <v>153</v>
+      </c>
+      <c r="B65" t="s">
+        <v>154</v>
+      </c>
+      <c r="C65" t="s">
         <v>155</v>
-      </c>
-      <c r="B65" t="s">
-        <v>156</v>
-      </c>
-      <c r="C65" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B66" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" t="s">
+        <v>158</v>
+      </c>
+      <c r="B67" t="s">
+        <v>159</v>
+      </c>
+      <c r="C67" t="s">
         <v>160</v>
       </c>
-      <c r="B67" t="s">
+      <c r="D67" t="s">
         <v>161</v>
       </c>
-      <c r="C67" t="s">
+      <c r="E67" t="s">
         <v>162</v>
-      </c>
-      <c r="D67" t="s">
-        <v>163</v>
-      </c>
-      <c r="E67" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B68" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" t="s">
+        <v>165</v>
+      </c>
+      <c r="B69" t="s">
+        <v>166</v>
+      </c>
+      <c r="C69" t="s">
         <v>167</v>
-      </c>
-      <c r="B69" t="s">
-        <v>168</v>
-      </c>
-      <c r="C69" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" t="s">
+        <v>168</v>
+      </c>
+      <c r="B70" t="s">
+        <v>169</v>
+      </c>
+      <c r="C70" t="s">
         <v>170</v>
-      </c>
-      <c r="B70" t="s">
-        <v>171</v>
-      </c>
-      <c r="C70" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" t="s">
+        <v>171</v>
+      </c>
+      <c r="B71" t="s">
+        <v>172</v>
+      </c>
+      <c r="C71" t="s">
         <v>173</v>
-      </c>
-      <c r="B71" t="s">
-        <v>174</v>
-      </c>
-      <c r="C71" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" t="s">
+        <v>174</v>
+      </c>
+      <c r="B72" t="s">
+        <v>175</v>
+      </c>
+      <c r="C72" t="s">
         <v>176</v>
-      </c>
-      <c r="B72" t="s">
-        <v>177</v>
-      </c>
-      <c r="C72" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" t="s">
+        <v>177</v>
+      </c>
+      <c r="B73" t="s">
+        <v>178</v>
+      </c>
+      <c r="C73" t="s">
         <v>179</v>
       </c>
-      <c r="B73" t="s">
+      <c r="D73" t="s">
         <v>180</v>
-      </c>
-      <c r="C73" t="s">
-        <v>181</v>
-      </c>
-      <c r="D73" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B74" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B75" t="s">
-        <v>185</v>
+        <v>382</v>
       </c>
       <c r="C75" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B76" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B77" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C77" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B78" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C78" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" t="s">
+        <v>191</v>
+      </c>
+      <c r="B79" t="s">
+        <v>192</v>
+      </c>
+      <c r="C79" t="s">
+        <v>193</v>
+      </c>
+      <c r="D79" t="s">
         <v>194</v>
-      </c>
-      <c r="B79" t="s">
-        <v>195</v>
-      </c>
-      <c r="C79" t="s">
-        <v>196</v>
-      </c>
-      <c r="D79" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B80" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="81" spans="1:7">
       <c r="A81" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B81" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="82" spans="1:7">
       <c r="A82" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B82" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C82" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="83" spans="1:7">
       <c r="A83" t="s">
+        <v>202</v>
+      </c>
+      <c r="B83" t="s">
+        <v>203</v>
+      </c>
+      <c r="C83" t="s">
+        <v>383</v>
+      </c>
+      <c r="D83" t="s">
+        <v>204</v>
+      </c>
+      <c r="E83" t="s">
         <v>205</v>
-      </c>
-      <c r="B83" t="s">
-        <v>206</v>
-      </c>
-      <c r="C83" t="s">
-        <v>354</v>
-      </c>
-      <c r="D83" t="s">
-        <v>207</v>
-      </c>
-      <c r="E83" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="84" spans="1:7">
       <c r="A84" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B84" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="85" spans="1:7">
       <c r="A85" t="s">
-        <v>211</v>
-      </c>
-      <c r="B85" t="s">
-        <v>212</v>
-      </c>
-      <c r="C85" t="s">
-        <v>213</v>
-      </c>
-      <c r="D85" t="s">
-        <v>214</v>
-      </c>
-      <c r="E85" t="s">
-        <v>215</v>
+        <v>374</v>
       </c>
     </row>
     <row r="86" spans="1:7">
       <c r="A86" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="B86" t="s">
-        <v>360</v>
+        <v>209</v>
+      </c>
+      <c r="C86" t="s">
+        <v>210</v>
+      </c>
+      <c r="D86" t="s">
+        <v>211</v>
+      </c>
+      <c r="E86" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="87" spans="1:7">
       <c r="A87" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B87" t="s">
-        <v>218</v>
-      </c>
-      <c r="C87" t="s">
-        <v>219</v>
+        <v>356</v>
       </c>
     </row>
     <row r="88" spans="1:7">
       <c r="A88" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B88" t="s">
-        <v>221</v>
+        <v>215</v>
+      </c>
+      <c r="C88" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="89" spans="1:7">
       <c r="A89" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="B89" t="s">
-        <v>223</v>
-      </c>
-      <c r="C89" t="s">
-        <v>224</v>
-      </c>
-      <c r="D89" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="90" spans="1:7">
       <c r="A90" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B90" t="s">
-        <v>361</v>
+        <v>220</v>
+      </c>
+      <c r="C90" t="s">
+        <v>221</v>
+      </c>
+      <c r="D90" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="91" spans="1:7">
       <c r="A91" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B91" t="s">
-        <v>228</v>
-      </c>
-      <c r="C91" t="s">
-        <v>229</v>
-      </c>
-      <c r="D91" t="s">
-        <v>230</v>
+        <v>357</v>
       </c>
     </row>
     <row r="92" spans="1:7">
       <c r="A92" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B92" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="C92" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="D92" t="s">
-        <v>234</v>
-      </c>
-      <c r="E92" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
     </row>
     <row r="93" spans="1:7">
       <c r="A93" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="B93" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="C93" t="s">
-        <v>238</v>
+        <v>230</v>
+      </c>
+      <c r="D93" t="s">
+        <v>231</v>
+      </c>
+      <c r="E93" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="94" spans="1:7">
       <c r="A94" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B94" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="C94" t="s">
-        <v>241</v>
-      </c>
-      <c r="D94" t="s">
-        <v>242</v>
-      </c>
-      <c r="E94" t="s">
-        <v>243</v>
-      </c>
-      <c r="F94" t="s">
-        <v>244</v>
-      </c>
-      <c r="G94" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
     </row>
     <row r="95" spans="1:7">
       <c r="A95" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="B95" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="C95" t="s">
-        <v>248</v>
+        <v>238</v>
+      </c>
+      <c r="D95" t="s">
+        <v>239</v>
+      </c>
+      <c r="E95" t="s">
+        <v>240</v>
+      </c>
+      <c r="F95" t="s">
+        <v>241</v>
+      </c>
+      <c r="G95" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="96" spans="1:7">
       <c r="A96" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="B96" t="s">
-        <v>250</v>
+        <v>387</v>
+      </c>
+      <c r="C96" t="s">
+        <v>244</v>
+      </c>
+      <c r="D96" t="s">
+        <v>245</v>
+      </c>
+      <c r="E96" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="97" spans="1:7">
       <c r="A97" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B97" t="s">
-        <v>252</v>
-      </c>
-      <c r="C97" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="98" spans="1:7">
       <c r="A98" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="B98" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C98" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="99" spans="1:7">
       <c r="A99" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="B99" t="s">
-        <v>258</v>
+        <v>252</v>
+      </c>
+      <c r="C99" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="100" spans="1:7">
       <c r="A100" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="B100" t="s">
-        <v>260</v>
-      </c>
-      <c r="C100" t="s">
-        <v>261</v>
-      </c>
-      <c r="D100" t="s">
-        <v>262</v>
-      </c>
-      <c r="E100" t="s">
-        <v>263</v>
-      </c>
-      <c r="F100" t="s">
-        <v>264</v>
-      </c>
-      <c r="G100" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
     </row>
     <row r="101" spans="1:7">
       <c r="A101" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="B101" t="s">
-        <v>267</v>
+        <v>257</v>
+      </c>
+      <c r="C101" t="s">
+        <v>258</v>
+      </c>
+      <c r="D101" t="s">
+        <v>259</v>
+      </c>
+      <c r="E101" t="s">
+        <v>260</v>
+      </c>
+      <c r="F101" t="s">
+        <v>261</v>
+      </c>
+      <c r="G101" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="102" spans="1:7">
       <c r="A102" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="B102" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="103" spans="1:7">
       <c r="A103" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B103" t="s">
-        <v>271</v>
-      </c>
-      <c r="C103" t="s">
-        <v>272</v>
-      </c>
-      <c r="D103" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="104" spans="1:7">
       <c r="A104" t="s">
-        <v>274</v>
+        <v>267</v>
+      </c>
+      <c r="B104" t="s">
+        <v>268</v>
+      </c>
+      <c r="C104" t="s">
+        <v>269</v>
+      </c>
+      <c r="D104" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="105" spans="1:7">
       <c r="A105" t="s">
-        <v>275</v>
+        <v>271</v>
+      </c>
+      <c r="B105" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="106" spans="1:7">
       <c r="A106" t="s">
-        <v>276</v>
-      </c>
-      <c r="B106" t="s">
-        <v>366</v>
+        <v>272</v>
       </c>
     </row>
     <row r="107" spans="1:7">
       <c r="A107" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B107" t="s">
-        <v>278</v>
-      </c>
-      <c r="C107" t="s">
-        <v>279</v>
+        <v>362</v>
       </c>
     </row>
     <row r="108" spans="1:7">
       <c r="A108" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="B108" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="C108" t="s">
-        <v>282</v>
-      </c>
-      <c r="D108" t="s">
-        <v>283</v>
-      </c>
-      <c r="E108" t="s">
-        <v>284</v>
-      </c>
-      <c r="F108" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
     </row>
     <row r="109" spans="1:7">
       <c r="A109" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="B109" t="s">
-        <v>287</v>
+        <v>278</v>
+      </c>
+      <c r="C109" t="s">
+        <v>279</v>
+      </c>
+      <c r="D109" t="s">
+        <v>377</v>
+      </c>
+      <c r="E109" t="s">
+        <v>280</v>
+      </c>
+      <c r="F109" t="s">
+        <v>281</v>
+      </c>
+      <c r="G109" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="110" spans="1:7">
       <c r="A110" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B110" t="s">
-        <v>355</v>
-      </c>
-      <c r="C110" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
     </row>
     <row r="111" spans="1:7">
       <c r="A111" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="B111" t="s">
-        <v>291</v>
+        <v>351</v>
+      </c>
+      <c r="C111" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="112" spans="1:7">
       <c r="A112" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="B112" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="C112" t="s">
-        <v>294</v>
-      </c>
-      <c r="D112" t="s">
-        <v>295</v>
+        <v>386</v>
       </c>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="B113" t="s">
-        <v>362</v>
+        <v>290</v>
       </c>
       <c r="C113" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="D113" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="B114" t="s">
-        <v>300</v>
+        <v>358</v>
       </c>
       <c r="C114" t="s">
-        <v>301</v>
+        <v>294</v>
+      </c>
+      <c r="D114" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="115" spans="1:4">
       <c r="A115" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="B115" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="C115" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
     </row>
     <row r="116" spans="1:4">
       <c r="A116" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="B116" t="s">
-        <v>306</v>
+        <v>300</v>
+      </c>
+      <c r="C116" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="B117" t="s">
-        <v>308</v>
-      </c>
-      <c r="C117" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
     </row>
     <row r="118" spans="1:4">
       <c r="A118" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="B118" t="s">
-        <v>311</v>
+        <v>305</v>
+      </c>
+      <c r="C118" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="119" spans="1:4">
       <c r="A119" t="s">
-        <v>364</v>
+        <v>307</v>
       </c>
       <c r="B119" t="s">
-        <v>363</v>
+        <v>308</v>
       </c>
     </row>
     <row r="120" spans="1:4">
       <c r="A120" t="s">
-        <v>312</v>
+        <v>360</v>
       </c>
       <c r="B120" t="s">
-        <v>313</v>
-      </c>
-      <c r="C120" t="s">
-        <v>314</v>
+        <v>359</v>
       </c>
     </row>
     <row r="121" spans="1:4">
       <c r="A121" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="B121" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="C121" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
     </row>
     <row r="122" spans="1:4">
       <c r="A122" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="B122" t="s">
-        <v>319</v>
+        <v>313</v>
+      </c>
+      <c r="C122" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="123" spans="1:4">
       <c r="A123" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="B123" t="s">
-        <v>321</v>
-      </c>
-      <c r="C123" t="s">
-        <v>365</v>
+        <v>316</v>
       </c>
     </row>
     <row r="124" spans="1:4">
       <c r="A124" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="B124" t="s">
-        <v>323</v>
+        <v>318</v>
+      </c>
+      <c r="C124" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="125" spans="1:4">
       <c r="A125" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B125" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="126" spans="1:4">
       <c r="A126" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="B126" t="s">
-        <v>327</v>
-      </c>
-      <c r="C126" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
     </row>
     <row r="127" spans="1:4">
       <c r="A127" t="s">
-        <v>329</v>
+        <v>323</v>
+      </c>
+      <c r="B127" t="s">
+        <v>324</v>
+      </c>
+      <c r="C127" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" t="s">
-        <v>330</v>
-      </c>
-      <c r="B128" t="s">
-        <v>331</v>
-      </c>
-      <c r="C128" t="s">
-        <v>332</v>
+        <v>373</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>333</v>
-      </c>
-      <c r="B129" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="B130" t="s">
-        <v>336</v>
+        <v>328</v>
+      </c>
+      <c r="C130" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="B131" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>372</v>
+        <v>332</v>
       </c>
       <c r="B132" t="s">
-        <v>375</v>
+        <v>333</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="B133" t="s">
-        <v>340</v>
-      </c>
-      <c r="C133" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
-        <v>342</v>
+        <v>368</v>
       </c>
       <c r="B134" t="s">
-        <v>343</v>
+        <v>371</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="B135" t="s">
-        <v>345</v>
+        <v>337</v>
+      </c>
+      <c r="C135" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" t="s">
+        <v>339</v>
+      </c>
+      <c r="B136" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" t="s">
+        <v>341</v>
+      </c>
+      <c r="B137" t="s">
+        <v>342</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moving all images locally
</commit_message>
<xml_diff>
--- a/LeagueSkins.xlsx
+++ b/LeagueSkins.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="393">
   <si>
     <t>Champion</t>
   </si>
@@ -1190,6 +1190,9 @@
   </si>
   <si>
     <t>Elementalist Lux</t>
+  </si>
+  <si>
+    <t>Kayn</t>
   </si>
 </sst>
 </file>
@@ -1529,10 +1532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J137"/>
+  <dimension ref="A1:J138"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2139,432 +2142,420 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" t="s">
-        <v>135</v>
-      </c>
-      <c r="B55" t="s">
-        <v>136</v>
+        <v>392</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B56" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" t="s">
-        <v>139</v>
+        <v>137</v>
+      </c>
+      <c r="B57" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" t="s">
-        <v>369</v>
+        <v>139</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" t="s">
-        <v>140</v>
-      </c>
-      <c r="B59" t="s">
-        <v>141</v>
-      </c>
-      <c r="C59" t="s">
-        <v>142</v>
-      </c>
-      <c r="D59" t="s">
-        <v>143</v>
+        <v>369</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B60" t="s">
-        <v>145</v>
+        <v>141</v>
+      </c>
+      <c r="C60" t="s">
+        <v>142</v>
+      </c>
+      <c r="D60" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B61" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B62" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B63" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B64" t="s">
-        <v>376</v>
+        <v>151</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B65" t="s">
-        <v>154</v>
-      </c>
-      <c r="C65" t="s">
-        <v>155</v>
+        <v>376</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B66" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C66" t="s">
-        <v>391</v>
+        <v>155</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B67" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C67" t="s">
-        <v>160</v>
-      </c>
-      <c r="D67" t="s">
-        <v>161</v>
-      </c>
-      <c r="E67" t="s">
-        <v>162</v>
+        <v>391</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B68" t="s">
-        <v>164</v>
+        <v>159</v>
+      </c>
+      <c r="C68" t="s">
+        <v>160</v>
+      </c>
+      <c r="D68" t="s">
+        <v>161</v>
+      </c>
+      <c r="E68" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B69" t="s">
-        <v>166</v>
-      </c>
-      <c r="C69" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B70" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C70" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B71" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C71" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B72" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C72" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B73" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C73" t="s">
-        <v>179</v>
-      </c>
-      <c r="D73" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B74" t="s">
-        <v>372</v>
+        <v>178</v>
+      </c>
+      <c r="C74" t="s">
+        <v>179</v>
+      </c>
+      <c r="D74" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B75" t="s">
-        <v>382</v>
-      </c>
-      <c r="C75" t="s">
-        <v>183</v>
+        <v>372</v>
       </c>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B76" t="s">
-        <v>350</v>
+        <v>382</v>
+      </c>
+      <c r="C76" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B77" t="s">
-        <v>186</v>
-      </c>
-      <c r="C77" t="s">
-        <v>187</v>
+        <v>350</v>
       </c>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B78" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C78" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B79" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C79" t="s">
-        <v>193</v>
-      </c>
-      <c r="D79" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B80" t="s">
-        <v>196</v>
+        <v>192</v>
+      </c>
+      <c r="C80" t="s">
+        <v>193</v>
+      </c>
+      <c r="D80" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="81" spans="1:7">
       <c r="A81" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B81" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="82" spans="1:7">
       <c r="A82" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B82" t="s">
-        <v>200</v>
-      </c>
-      <c r="C82" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="83" spans="1:7">
       <c r="A83" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B83" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C83" t="s">
-        <v>383</v>
-      </c>
-      <c r="D83" t="s">
-        <v>204</v>
-      </c>
-      <c r="E83" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="84" spans="1:7">
       <c r="A84" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B84" t="s">
-        <v>207</v>
+        <v>203</v>
+      </c>
+      <c r="C84" t="s">
+        <v>383</v>
+      </c>
+      <c r="D84" t="s">
+        <v>204</v>
+      </c>
+      <c r="E84" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="85" spans="1:7">
       <c r="A85" t="s">
-        <v>374</v>
+        <v>206</v>
+      </c>
+      <c r="B85" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="86" spans="1:7">
       <c r="A86" t="s">
-        <v>208</v>
-      </c>
-      <c r="B86" t="s">
-        <v>209</v>
-      </c>
-      <c r="C86" t="s">
-        <v>210</v>
-      </c>
-      <c r="D86" t="s">
-        <v>211</v>
-      </c>
-      <c r="E86" t="s">
-        <v>212</v>
+        <v>374</v>
       </c>
     </row>
     <row r="87" spans="1:7">
       <c r="A87" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B87" t="s">
-        <v>356</v>
+        <v>209</v>
+      </c>
+      <c r="C87" t="s">
+        <v>210</v>
+      </c>
+      <c r="D87" t="s">
+        <v>211</v>
+      </c>
+      <c r="E87" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="88" spans="1:7">
       <c r="A88" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B88" t="s">
-        <v>215</v>
-      </c>
-      <c r="C88" t="s">
-        <v>216</v>
+        <v>356</v>
       </c>
     </row>
     <row r="89" spans="1:7">
       <c r="A89" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B89" t="s">
-        <v>218</v>
+        <v>215</v>
+      </c>
+      <c r="C89" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="90" spans="1:7">
       <c r="A90" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B90" t="s">
-        <v>220</v>
-      </c>
-      <c r="C90" t="s">
-        <v>221</v>
-      </c>
-      <c r="D90" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="91" spans="1:7">
       <c r="A91" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B91" t="s">
-        <v>357</v>
+        <v>220</v>
+      </c>
+      <c r="C91" t="s">
+        <v>221</v>
+      </c>
+      <c r="D91" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="92" spans="1:7">
       <c r="A92" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B92" t="s">
-        <v>225</v>
-      </c>
-      <c r="C92" t="s">
-        <v>226</v>
-      </c>
-      <c r="D92" t="s">
-        <v>227</v>
+        <v>357</v>
       </c>
     </row>
     <row r="93" spans="1:7">
       <c r="A93" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B93" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C93" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D93" t="s">
-        <v>231</v>
-      </c>
-      <c r="E93" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="94" spans="1:7">
       <c r="A94" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B94" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="C94" t="s">
-        <v>235</v>
+        <v>230</v>
+      </c>
+      <c r="D94" t="s">
+        <v>231</v>
+      </c>
+      <c r="E94" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="95" spans="1:7">
       <c r="A95" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B95" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C95" t="s">
-        <v>238</v>
-      </c>
-      <c r="D95" t="s">
-        <v>239</v>
-      </c>
-      <c r="E95" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="F95" t="s">
         <v>241</v>
@@ -2575,74 +2566,74 @@
     </row>
     <row r="96" spans="1:7">
       <c r="A96" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B96" t="s">
-        <v>387</v>
+        <v>237</v>
       </c>
       <c r="C96" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="D96" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="E96" t="s">
-        <v>388</v>
+        <v>240</v>
       </c>
     </row>
     <row r="97" spans="1:7">
       <c r="A97" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B97" t="s">
-        <v>247</v>
+        <v>387</v>
+      </c>
+      <c r="C97" t="s">
+        <v>244</v>
+      </c>
+      <c r="D97" t="s">
+        <v>245</v>
+      </c>
+      <c r="E97" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="98" spans="1:7">
       <c r="A98" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B98" t="s">
-        <v>249</v>
-      </c>
-      <c r="C98" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="99" spans="1:7">
       <c r="A99" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B99" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C99" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="100" spans="1:7">
       <c r="A100" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B100" t="s">
-        <v>255</v>
+        <v>252</v>
+      </c>
+      <c r="C100" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="101" spans="1:7">
       <c r="A101" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B101" t="s">
-        <v>257</v>
-      </c>
-      <c r="C101" t="s">
-        <v>258</v>
-      </c>
-      <c r="D101" t="s">
-        <v>259</v>
-      </c>
-      <c r="E101" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="F101" t="s">
         <v>261</v>
@@ -2653,81 +2644,81 @@
     </row>
     <row r="102" spans="1:7">
       <c r="A102" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="B102" t="s">
-        <v>264</v>
+        <v>257</v>
+      </c>
+      <c r="C102" t="s">
+        <v>258</v>
+      </c>
+      <c r="D102" t="s">
+        <v>259</v>
+      </c>
+      <c r="E102" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="103" spans="1:7">
       <c r="A103" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B103" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="104" spans="1:7">
       <c r="A104" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B104" t="s">
-        <v>268</v>
-      </c>
-      <c r="C104" t="s">
-        <v>269</v>
-      </c>
-      <c r="D104" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="105" spans="1:7">
       <c r="A105" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B105" t="s">
-        <v>384</v>
+        <v>268</v>
+      </c>
+      <c r="C105" t="s">
+        <v>269</v>
+      </c>
+      <c r="D105" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="106" spans="1:7">
       <c r="A106" t="s">
-        <v>272</v>
+        <v>271</v>
+      </c>
+      <c r="B106" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="107" spans="1:7">
       <c r="A107" t="s">
-        <v>273</v>
-      </c>
-      <c r="B107" t="s">
-        <v>362</v>
+        <v>272</v>
       </c>
     </row>
     <row r="108" spans="1:7">
       <c r="A108" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B108" t="s">
-        <v>275</v>
-      </c>
-      <c r="C108" t="s">
-        <v>276</v>
+        <v>362</v>
       </c>
     </row>
     <row r="109" spans="1:7">
       <c r="A109" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B109" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C109" t="s">
-        <v>279</v>
-      </c>
-      <c r="D109" t="s">
-        <v>377</v>
-      </c>
-      <c r="E109" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="F109" t="s">
         <v>281</v>
@@ -2738,264 +2729,281 @@
     </row>
     <row r="110" spans="1:7">
       <c r="A110" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="B110" t="s">
-        <v>284</v>
+        <v>278</v>
+      </c>
+      <c r="C110" t="s">
+        <v>279</v>
+      </c>
+      <c r="D110" t="s">
+        <v>377</v>
+      </c>
+      <c r="E110" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="111" spans="1:7">
       <c r="A111" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B111" t="s">
-        <v>351</v>
-      </c>
-      <c r="C111" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="112" spans="1:7">
       <c r="A112" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B112" t="s">
-        <v>288</v>
+        <v>351</v>
       </c>
       <c r="C112" t="s">
-        <v>386</v>
+        <v>286</v>
       </c>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B113" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C113" t="s">
-        <v>291</v>
-      </c>
-      <c r="D113" t="s">
-        <v>292</v>
+        <v>386</v>
       </c>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B114" t="s">
-        <v>358</v>
+        <v>290</v>
       </c>
       <c r="C114" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D114" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="115" spans="1:4">
       <c r="A115" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B115" t="s">
-        <v>297</v>
+        <v>358</v>
       </c>
       <c r="C115" t="s">
-        <v>298</v>
+        <v>294</v>
+      </c>
+      <c r="D115" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="116" spans="1:4">
       <c r="A116" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B116" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C116" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B117" t="s">
-        <v>303</v>
+        <v>300</v>
+      </c>
+      <c r="C117" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="118" spans="1:4">
       <c r="A118" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B118" t="s">
-        <v>305</v>
-      </c>
-      <c r="C118" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="119" spans="1:4">
       <c r="A119" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B119" t="s">
-        <v>308</v>
+        <v>305</v>
+      </c>
+      <c r="C119" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="120" spans="1:4">
       <c r="A120" t="s">
-        <v>360</v>
+        <v>307</v>
       </c>
       <c r="B120" t="s">
-        <v>359</v>
+        <v>308</v>
       </c>
     </row>
     <row r="121" spans="1:4">
       <c r="A121" t="s">
-        <v>309</v>
+        <v>360</v>
       </c>
       <c r="B121" t="s">
-        <v>310</v>
-      </c>
-      <c r="C121" t="s">
-        <v>311</v>
+        <v>359</v>
       </c>
     </row>
     <row r="122" spans="1:4">
       <c r="A122" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B122" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C122" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="123" spans="1:4">
       <c r="A123" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B123" t="s">
-        <v>316</v>
+        <v>313</v>
+      </c>
+      <c r="C123" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="124" spans="1:4">
       <c r="A124" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B124" t="s">
-        <v>318</v>
-      </c>
-      <c r="C124" t="s">
-        <v>361</v>
+        <v>316</v>
       </c>
     </row>
     <row r="125" spans="1:4">
       <c r="A125" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B125" t="s">
-        <v>320</v>
+        <v>318</v>
+      </c>
+      <c r="C125" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="126" spans="1:4">
       <c r="A126" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B126" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="127" spans="1:4">
       <c r="A127" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B127" t="s">
-        <v>324</v>
-      </c>
-      <c r="C127" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" t="s">
-        <v>373</v>
+        <v>323</v>
+      </c>
+      <c r="B128" t="s">
+        <v>324</v>
+      </c>
+      <c r="C128" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>326</v>
+        <v>373</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>327</v>
-      </c>
-      <c r="B130" t="s">
-        <v>328</v>
-      </c>
-      <c r="C130" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B131" t="s">
-        <v>331</v>
+        <v>328</v>
+      </c>
+      <c r="C131" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B132" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B133" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
-        <v>368</v>
+        <v>334</v>
       </c>
       <c r="B134" t="s">
-        <v>371</v>
+        <v>335</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
-        <v>336</v>
+        <v>368</v>
       </c>
       <c r="B135" t="s">
-        <v>337</v>
-      </c>
-      <c r="C135" t="s">
-        <v>338</v>
+        <v>371</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B136" t="s">
-        <v>340</v>
+        <v>337</v>
+      </c>
+      <c r="C136" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" t="s">
+        <v>339</v>
+      </c>
+      <c r="B137" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" t="s">
         <v>341</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B138" t="s">
         <v>342</v>
       </c>
     </row>

</xml_diff>